<commit_message>
Erster Durchstich Read und Open
</commit_message>
<xml_diff>
--- a/Fertigstellungsgrad Statements.xlsx
+++ b/Fertigstellungsgrad Statements.xlsx
@@ -536,7 +536,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,7 +551,7 @@
       </c>
       <c r="B1" s="4">
         <f>SUM(B2:B50)/49</f>
-        <v>0.19</v>
+        <v>0.20183673469387753</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -595,11 +595,11 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="5">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -819,11 +819,11 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="5">
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Verschiedene Korrekturen, um die Tests wieder zu durchlaufen
</commit_message>
<xml_diff>
--- a/Fertigstellungsgrad Statements.xlsx
+++ b/Fertigstellungsgrad Statements.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cobolj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flaechsig\git\cobolj\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -533,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,32 +545,42 @@
     <col min="2" max="2" width="11.5546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B1" s="4">
         <f>SUM(B2:B50)/49</f>
-        <v>0.20183673469387753</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.21204081632653063</v>
+      </c>
+      <c r="C1" s="4">
+        <f>SUM(C2:C50)/49</f>
+        <v>0.30612244897959184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -578,7 +588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -586,7 +596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -594,31 +604,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="5">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -626,7 +645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -634,23 +653,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -658,7 +683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -666,7 +691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -674,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -682,7 +707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -690,7 +715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -698,7 +723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -706,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -714,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -722,7 +747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -730,7 +755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -738,15 +763,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -754,7 +782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -762,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -770,7 +798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -778,39 +806,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.5</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="5">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -818,15 +858,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="5">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -834,7 +877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -842,7 +885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -850,7 +893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -858,7 +901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -866,7 +909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -874,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -882,7 +925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -890,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -898,15 +941,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -914,15 +960,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="5">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Write-Statement und viele Anpassungen
</commit_message>
<xml_diff>
--- a/Fertigstellungsgrad Statements.xlsx
+++ b/Fertigstellungsgrad Statements.xlsx
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,6 +566,7 @@
         <v>0.3</v>
       </c>
       <c r="C2">
+        <f>IF(B2&gt;0,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -577,6 +578,7 @@
         <v>0.67</v>
       </c>
       <c r="C3">
+        <f>IF(B3&gt;0,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -587,6 +589,10 @@
       <c r="B4" s="5">
         <v>0</v>
       </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C50" si="0">IF(B4&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -595,6 +601,10 @@
       <c r="B5" s="5">
         <v>0</v>
       </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -603,6 +613,10 @@
       <c r="B6" s="5">
         <v>0</v>
       </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -612,6 +626,7 @@
         <v>0.25</v>
       </c>
       <c r="C7">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -623,6 +638,7 @@
         <v>1</v>
       </c>
       <c r="C8">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -634,6 +650,7 @@
         <v>1</v>
       </c>
       <c r="C9">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -644,6 +661,10 @@
       <c r="B10" s="5">
         <v>0</v>
       </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -652,6 +673,10 @@
       <c r="B11" s="5">
         <v>0</v>
       </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -661,6 +686,7 @@
         <v>0.5</v>
       </c>
       <c r="C12">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -672,6 +698,7 @@
         <v>1</v>
       </c>
       <c r="C13">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -682,6 +709,10 @@
       <c r="B14" s="5">
         <v>0</v>
       </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -690,6 +721,10 @@
       <c r="B15" s="5">
         <v>0</v>
       </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -698,6 +733,10 @@
       <c r="B16" s="5">
         <v>0</v>
       </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -706,6 +745,10 @@
       <c r="B17" s="5">
         <v>0</v>
       </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -714,6 +757,10 @@
       <c r="B18" s="5">
         <v>0</v>
       </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -722,6 +769,10 @@
       <c r="B19" s="5">
         <v>0</v>
       </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -730,6 +781,10 @@
       <c r="B20" s="5">
         <v>0</v>
       </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -738,6 +793,10 @@
       <c r="B21" s="5">
         <v>0</v>
       </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -746,6 +805,10 @@
       <c r="B22" s="5">
         <v>0</v>
       </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -754,6 +817,10 @@
       <c r="B23" s="5">
         <v>0</v>
       </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
@@ -762,6 +829,10 @@
       <c r="B24" s="5">
         <v>0</v>
       </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
@@ -771,6 +842,7 @@
         <v>1</v>
       </c>
       <c r="C25">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -781,6 +853,10 @@
       <c r="B26" s="5">
         <v>0</v>
       </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -789,6 +865,10 @@
       <c r="B27" s="5">
         <v>0</v>
       </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -797,6 +877,10 @@
       <c r="B28" s="5">
         <v>0</v>
       </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
@@ -805,6 +889,10 @@
       <c r="B29" s="5">
         <v>0</v>
       </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
@@ -814,6 +902,7 @@
         <v>0.5</v>
       </c>
       <c r="C30">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -825,6 +914,7 @@
         <v>1</v>
       </c>
       <c r="C31">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -836,6 +926,7 @@
         <v>0.5</v>
       </c>
       <c r="C32">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -847,6 +938,7 @@
         <v>0.67</v>
       </c>
       <c r="C33">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -857,6 +949,10 @@
       <c r="B34" s="5">
         <v>0</v>
       </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
@@ -866,6 +962,7 @@
         <v>0.33</v>
       </c>
       <c r="C35">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -876,6 +973,10 @@
       <c r="B36" s="5">
         <v>0</v>
       </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
@@ -884,6 +985,10 @@
       <c r="B37" s="5">
         <v>0</v>
       </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -892,6 +997,10 @@
       <c r="B38" s="5">
         <v>0</v>
       </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
@@ -900,6 +1009,10 @@
       <c r="B39" s="5">
         <v>0</v>
       </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
@@ -908,6 +1021,10 @@
       <c r="B40" s="5">
         <v>0</v>
       </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
@@ -916,6 +1033,10 @@
       <c r="B41" s="5">
         <v>0</v>
       </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
@@ -924,6 +1045,10 @@
       <c r="B42" s="5">
         <v>0</v>
       </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
@@ -932,6 +1057,10 @@
       <c r="B43" s="5">
         <v>0</v>
       </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
@@ -940,6 +1069,10 @@
       <c r="B44" s="5">
         <v>0</v>
       </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
@@ -949,6 +1082,7 @@
         <v>1</v>
       </c>
       <c r="C45">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -959,6 +1093,10 @@
       <c r="B46" s="5">
         <v>0</v>
       </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
@@ -968,6 +1106,7 @@
         <v>0.67</v>
       </c>
       <c r="C47">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -978,20 +1117,32 @@
       <c r="B48" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B49" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B50" s="5">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Klassen in die richtigen Packages veschoben (Refactoring)
</commit_message>
<xml_diff>
--- a/Fertigstellungsgrad Statements.xlsx
+++ b/Fertigstellungsgrad Statements.xlsx
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,11 +551,11 @@
       </c>
       <c r="B1" s="4">
         <f>SUM(B2:B50)/49</f>
-        <v>0.21204081632653063</v>
+        <v>0.21612244897959185</v>
       </c>
       <c r="C1" s="4">
         <f>SUM(C2:C50)/49</f>
-        <v>0.30612244897959184</v>
+        <v>0.32653061224489793</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1139,11 +1139,11 @@
         <v>48</v>
       </c>
       <c r="B50" s="5">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Erste Version des String-Statements
</commit_message>
<xml_diff>
--- a/Fertigstellungsgrad Statements.xlsx
+++ b/Fertigstellungsgrad Statements.xlsx
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,11 +551,11 @@
       </c>
       <c r="B1" s="4">
         <f>SUM(B2:B50)/49</f>
-        <v>0.21612244897959185</v>
+        <v>0.22020408163265304</v>
       </c>
       <c r="C1" s="4">
         <f>SUM(C2:C50)/49</f>
-        <v>0.32653061224489793</v>
+        <v>0.34693877551020408</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1087,15 +1087,15 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="5">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1135,7 +1135,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B50" s="5">

</xml_diff>

<commit_message>
Erweiterung String-Statement um die Overflow-Phrasen
</commit_message>
<xml_diff>
--- a/Fertigstellungsgrad Statements.xlsx
+++ b/Fertigstellungsgrad Statements.xlsx
@@ -536,7 +536,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,7 +551,7 @@
       </c>
       <c r="B1" s="4">
         <f>SUM(B2:B50)/49</f>
-        <v>0.22020408163265304</v>
+        <v>0.22224489795918367</v>
       </c>
       <c r="C1" s="4">
         <f>SUM(C2:C50)/49</f>
@@ -1091,7 +1091,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="5">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C46">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Weitere Ergänzungen für das String-Statement
</commit_message>
<xml_diff>
--- a/Fertigstellungsgrad Statements.xlsx
+++ b/Fertigstellungsgrad Statements.xlsx
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,7 +551,7 @@
       </c>
       <c r="B1" s="4">
         <f>SUM(B2:B50)/49</f>
-        <v>0.22224489795918367</v>
+        <v>0.23653061224489796</v>
       </c>
       <c r="C1" s="4">
         <f>SUM(C2:C50)/49</f>
@@ -1087,11 +1087,11 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="5">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="C46">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Aufruf der konreten Statement-Visitor verallgemeinert, dass keine Anpassung beim Hinzufügen weiterer Statements notwendig wird
</commit_message>
<xml_diff>
--- a/Fertigstellungsgrad Statements.xlsx
+++ b/Fertigstellungsgrad Statements.xlsx
@@ -535,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
@@ -551,7 +551,7 @@
       </c>
       <c r="B1" s="4">
         <f>SUM(B2:B50)/49</f>
-        <v>0.23653061224489796</v>
+        <v>0.22632653061224489</v>
       </c>
       <c r="C1" s="4">
         <f>SUM(C2:C50)/49</f>
@@ -1075,11 +1075,11 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C45">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Call-Statement (1 von 5) implementiert
</commit_message>
<xml_diff>
--- a/Fertigstellungsgrad Statements.xlsx
+++ b/Fertigstellungsgrad Statements.xlsx
@@ -536,7 +536,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,11 +551,11 @@
       </c>
       <c r="B1" s="4">
         <f>SUM(B2:B50)/49</f>
-        <v>0.24673469387755101</v>
+        <v>0.25081632653061225</v>
       </c>
       <c r="C1" s="4">
         <f>SUM(C2:C50)/49</f>
-        <v>0.36734693877551022</v>
+        <v>0.38775510204081631</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -595,15 +595,15 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Größerer Umbau für die Einführung von Occurs (nocht nicht abgeschlossen)
</commit_message>
<xml_diff>
--- a/Fertigstellungsgrad Statements.xlsx
+++ b/Fertigstellungsgrad Statements.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>acceptStatement</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>Statement</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>File</t>
   </si>
 </sst>
 </file>
@@ -533,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,7 +551,7 @@
     <col min="2" max="2" width="11.5546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>49</v>
       </c>
@@ -558,7 +564,7 @@
         <v>0.38775510204081631</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -570,7 +576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -582,7 +588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -594,7 +600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -606,7 +612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -618,7 +624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -629,8 +635,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -642,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -654,7 +663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -665,8 +674,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -678,7 +690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -690,7 +702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
@@ -702,7 +714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -714,7 +726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -726,7 +738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -930,7 +942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>31</v>
       </c>
@@ -942,7 +954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -954,7 +966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -966,7 +978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -978,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -990,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -1001,8 +1013,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -1014,7 +1029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -1026,7 +1041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -1038,7 +1053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -1050,7 +1065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -1061,8 +1076,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -1073,8 +1091,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
@@ -1086,7 +1107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>44</v>
       </c>
@@ -1098,7 +1119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
@@ -1110,7 +1131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -1120,6 +1141,9 @@
       <c r="C48">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
GoTo (ohne Altered) implementiert
</commit_message>
<xml_diff>
--- a/Fertigstellungsgrad Statements.xlsx
+++ b/Fertigstellungsgrad Statements.xlsx
@@ -542,7 +542,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -557,11 +557,11 @@
       </c>
       <c r="B1" s="4">
         <f>SUM(B2:B50)/49</f>
-        <v>0.25183673469387757</v>
+        <v>0.27224489795918361</v>
       </c>
       <c r="C1" s="4">
         <f>SUM(C2:C50)/49</f>
-        <v>0.38775510204081631</v>
+        <v>0.40816326530612246</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -839,11 +839,11 @@
         <v>22</v>
       </c>
       <c r="B24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Imports optimiert. Doku angepasst
</commit_message>
<xml_diff>
--- a/Fertigstellungsgrad Statements.xlsx
+++ b/Fertigstellungsgrad Statements.xlsx
@@ -542,7 +542,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -835,7 +835,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="5">

</xml_diff>